<commit_message>
playing with extract_phase. potential to break program. have ided problem with holes in dataset
</commit_message>
<xml_diff>
--- a/Tests/1/Test_SingleRun1.xlsx
+++ b/Tests/1/Test_SingleRun1.xlsx
@@ -191,6 +191,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -326,8 +327,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,10 +342,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -665,55 +666,55 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="28"/>
       <c r="C2">
         <v>17875.075000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="24">
         <v>8554.2999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="25">
         <v>2770</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="12">
         <v>0.78019999999999978</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="6">
         <v>1.0394621801631903</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="7">
         <v>60</v>
       </c>
@@ -987,8 +988,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,10 +1005,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="28"/>
       <c r="C2">
         <v>17875.075000000001</v>
       </c>
@@ -1024,10 +1025,10 @@
       <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3">
         <v>8554.2999999999993</v>
       </c>
@@ -1044,10 +1045,10 @@
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4">
         <v>2770</v>
       </c>
@@ -1064,10 +1065,10 @@
       <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="12">
         <v>0.78019999999999978</v>
       </c>
@@ -1084,19 +1085,19 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="6">
         <v>1.0394621801631903</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="7">
         <v>60</v>
       </c>
@@ -1113,10 +1114,10 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="20">
         <v>45</v>
       </c>
@@ -1133,10 +1134,10 @@
       <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="30"/>
+      <c r="B9" s="32"/>
       <c r="C9">
         <f>C16+C10</f>
         <v>2.1162648926430907</v>
@@ -1154,10 +1155,10 @@
       <c r="N9" s="20"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="30"/>
       <c r="C10">
         <f>60*(C13-(C22/C21)*EXP(-1*C21*C8))/C2/C7</f>
         <v>0.6708723283302227</v>
@@ -1175,10 +1176,10 @@
       <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="30"/>
       <c r="C11">
         <f>C16/C9</f>
         <v>0.6829922706451258</v>
@@ -1193,10 +1194,10 @@
       <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="30"/>
       <c r="C12">
         <f>C9*C17/(3*0.693)</f>
         <v>21.280439961769162</v>
@@ -1214,10 +1215,10 @@
       <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="21">
         <f>(C3+C4)/C5</f>
         <v>14514.611638041531</v>
@@ -1235,7 +1236,7 @@
       <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -1257,12 +1258,12 @@
       <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="21">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20"/>
@@ -1277,7 +1278,7 @@
       <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="26" t="s">
         <v>21</v>
       </c>
@@ -1298,8 +1299,8 @@
       <c r="N16" s="20"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="21">
@@ -1319,8 +1320,8 @@
       <c r="N17" s="20"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -1340,8 +1341,8 @@
       <c r="N18" s="20"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="21">
@@ -1361,8 +1362,8 @@
       <c r="N19" s="20"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="21">
@@ -1382,8 +1383,8 @@
       <c r="N20" s="20"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="21">
@@ -1403,8 +1404,8 @@
       <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="21">
@@ -1424,7 +1425,7 @@
       <c r="N22" s="20"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="29" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="26" t="s">
@@ -1446,7 +1447,7 @@
       <c r="N23" s="20"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="26" t="s">
         <v>38</v>
       </c>
@@ -1466,7 +1467,7 @@
       <c r="N24" s="20"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="26" t="s">
         <v>21</v>
       </c>
@@ -1487,8 +1488,8 @@
       <c r="N25" s="20"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="29"/>
+      <c r="B26" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="21">
@@ -1508,8 +1509,8 @@
       <c r="N26" s="20"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C27">
@@ -1529,8 +1530,8 @@
       <c r="N27" s="20"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="29"/>
+      <c r="B28" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="21">
@@ -1550,8 +1551,8 @@
       <c r="N28" s="20"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="31" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="21">
@@ -1571,8 +1572,8 @@
       <c r="N29" s="20"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="21">
@@ -1592,8 +1593,8 @@
       <c r="N30" s="20"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="31" t="s">
+      <c r="A31" s="29"/>
+      <c r="B31" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="21">
@@ -1613,7 +1614,7 @@
       <c r="N31" s="20"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="26" t="s">
@@ -1624,7 +1625,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="26" t="s">
         <v>38</v>
       </c>
@@ -1644,7 +1645,7 @@
       <c r="N33" s="10"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="26" t="s">
         <v>21</v>
       </c>
@@ -1665,8 +1666,8 @@
       <c r="N34" s="20"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="21">
@@ -1686,8 +1687,8 @@
       <c r="N35" s="10"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="31" t="s">
+      <c r="A36" s="29"/>
+      <c r="B36" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C36">
@@ -1707,8 +1708,8 @@
       <c r="N36" s="10"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="31" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="21">
@@ -1728,8 +1729,8 @@
       <c r="N37" s="10"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="31" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="21">
@@ -1749,8 +1750,8 @@
       <c r="N38" s="10"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="31" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C39" s="21">
@@ -1770,8 +1771,8 @@
       <c r="N39" s="10"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="31" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="21">

</xml_diff>

<commit_message>
finished implementing fuzzy use of xs to point to indexs
</commit_message>
<xml_diff>
--- a/Tests/1/Test_SingleRun1.xlsx
+++ b/Tests/1/Test_SingleRun1.xlsx
@@ -649,8 +649,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,8 +988,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N353"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +1243,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="21">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="20"/>
@@ -1263,7 +1263,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="21">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20"/>
@@ -1432,7 +1432,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -1621,7 +1621,7 @@
         <v>37</v>
       </c>
       <c r="C32" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>